<commit_message>
Imported Upstream version 2.5
</commit_message>
<xml_diff>
--- a/src/site/resources/images/whichjar.xlsx
+++ b/src/site/resources/images/whichjar.xlsx
@@ -209,7 +209,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
-            <a:t>(log4j-1.2-api-2.1.jar)</a:t>
+            <a:t>(log4j-1.2-api-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -273,7 +273,7 @@
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900"/>
-            <a:t>2.1</a:t>
+            <a:t>2.x</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" baseline="0"/>
@@ -284,7 +284,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" baseline="0"/>
-            <a:t>(log4j-core-2.1.jar)</a:t>
+            <a:t>(log4j-core-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900"/>
         </a:p>
@@ -340,7 +340,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
-            <a:t>Log4J 2.1</a:t>
+            <a:t>Log4J 2.x</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
@@ -351,7 +351,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
-            <a:t>(log4j-api-2.1.jar)</a:t>
+            <a:t>(log4j-api-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -419,7 +419,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
-            <a:t>(log4j-slf4j-impl-2.1.jar)</a:t>
+            <a:t>(log4j-slf4j-impl-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -678,7 +678,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
-            <a:t>(log4j-jcl-2.1.jar)</a:t>
+            <a:t>(log4j-jcl-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -843,7 +843,7 @@
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
-            <a:t>2.1</a:t>
+            <a:t>2.x</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
@@ -854,7 +854,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
-            <a:t>(log4j-api-2.1.jar)</a:t>
+            <a:t>(log4j-api-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -1227,7 +1227,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
-            <a:t>(log4j-jul-2.1.jar)</a:t>
+            <a:t>(log4j-jul-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -1560,7 +1560,7 @@
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
-            <a:t>2.1</a:t>
+            <a:t>2.x</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
@@ -1571,7 +1571,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
-            <a:t>(log4j-api-2.1.jar)</a:t>
+            <a:t>(log4j-api-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -1741,7 +1741,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
-            <a:t>(log4j-to-slf4j-2.1.jar)</a:t>
+            <a:t>(log4j-to-slf4j-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -2187,7 +2187,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2206,7 +2206,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>